<commit_message>
[CC] correction of the reference values
</commit_message>
<xml_diff>
--- a/mosqito/tests/roughness/data/Test_fc_1000.xlsx
+++ b/mosqito/tests/roughness/data/Test_fc_1000.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Salomé\MoSQITo_oo\mosqito\tests\roughness\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Salomé\MoSQIToGUI\mosqito\tests\roughness\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2619A541-E131-4EFE-B689-0A3A54442B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58F30F7-5BDE-488D-B6F6-5A7756965055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F0CF267-26BD-4373-9BDF-601610C10383}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Roughness calculation according to Daniel and Weber method </t>
   </si>
@@ -51,124 +51,148 @@
     <t>R</t>
   </si>
   <si>
-    <t>11.210676</t>
-  </si>
-  <si>
-    <t>37.089394</t>
-  </si>
-  <si>
-    <t>42.61789</t>
-  </si>
-  <si>
-    <t>45.603157</t>
-  </si>
-  <si>
-    <t>48.968876</t>
-  </si>
-  <si>
-    <t>52.295155</t>
-  </si>
-  <si>
-    <t>56.306377</t>
-  </si>
-  <si>
-    <t>60.619404</t>
-  </si>
-  <si>
-    <t>65.2607</t>
-  </si>
-  <si>
-    <t>74.59246</t>
-  </si>
-  <si>
-    <t>80.285446</t>
-  </si>
-  <si>
-    <t>86.17377</t>
-  </si>
-  <si>
-    <t>90.73637</t>
-  </si>
-  <si>
-    <t>96.5827</t>
-  </si>
-  <si>
-    <t>102.80353</t>
-  </si>
-  <si>
-    <t>108.52951</t>
-  </si>
-  <si>
-    <t>115.82172</t>
-  </si>
-  <si>
-    <t>125.62914</t>
-  </si>
-  <si>
-    <t>143.09247</t>
-  </si>
-  <si>
-    <t>329.7389</t>
-  </si>
-  <si>
-    <t>0.1014365</t>
-  </si>
-  <si>
-    <t>0.587882</t>
-  </si>
-  <si>
-    <t>0.7035962</t>
-  </si>
-  <si>
-    <t>0.77971196</t>
-  </si>
-  <si>
-    <t>0.8351465</t>
-  </si>
-  <si>
-    <t>0.88716906</t>
-  </si>
-  <si>
-    <t>0.94240147</t>
-  </si>
-  <si>
-    <t>0.9765243</t>
-  </si>
-  <si>
-    <t>1.0035429</t>
-  </si>
-  <si>
-    <t>0.9920012</t>
-  </si>
-  <si>
-    <t>0.9620685</t>
-  </si>
-  <si>
-    <t>0.9228101</t>
-  </si>
-  <si>
-    <t>0.86589915</t>
-  </si>
-  <si>
-    <t>0.7991257</t>
-  </si>
-  <si>
-    <t>0.7334436</t>
-  </si>
-  <si>
-    <t>0.66763395</t>
-  </si>
-  <si>
-    <t>0.5944383</t>
-  </si>
-  <si>
-    <t>0.51341456</t>
-  </si>
-  <si>
-    <t>0.4172414</t>
-  </si>
-  <si>
-    <t>0.10044643</t>
+    <t>11.087001</t>
+  </si>
+  <si>
+    <t>13.655874</t>
+  </si>
+  <si>
+    <t>17.425774</t>
+  </si>
+  <si>
+    <t>22.323097</t>
+  </si>
+  <si>
+    <t>28.37367</t>
+  </si>
+  <si>
+    <t>34.94905</t>
+  </si>
+  <si>
+    <t>42.370758</t>
+  </si>
+  <si>
+    <t>49.96757</t>
+  </si>
+  <si>
+    <t>56.425716</t>
+  </si>
+  <si>
+    <t>63.209957</t>
+  </si>
+  <si>
+    <t>69.42832</t>
+  </si>
+  <si>
+    <t>74.194626</t>
+  </si>
+  <si>
+    <t>81.15967</t>
+  </si>
+  <si>
+    <t>87.05505</t>
+  </si>
+  <si>
+    <t>95.19742</t>
+  </si>
+  <si>
+    <t>103.28752</t>
+  </si>
+  <si>
+    <t>112.92756</t>
+  </si>
+  <si>
+    <t>137.10373</t>
+  </si>
+  <si>
+    <t>160.75127</t>
+  </si>
+  <si>
+    <t>193.66571</t>
+  </si>
+  <si>
+    <t>220.964</t>
+  </si>
+  <si>
+    <t>246.33324</t>
+  </si>
+  <si>
+    <t>284.3601</t>
+  </si>
+  <si>
+    <t>332.1115</t>
+  </si>
+  <si>
+    <t>0.10113691</t>
+  </si>
+  <si>
+    <t>0.13728729</t>
+  </si>
+  <si>
+    <t>0.19609652</t>
+  </si>
+  <si>
+    <t>0.27899456</t>
+  </si>
+  <si>
+    <t>0.39539358</t>
+  </si>
+  <si>
+    <t>0.5409575</t>
+  </si>
+  <si>
+    <t>0.7005437</t>
+  </si>
+  <si>
+    <t>0.8453598</t>
+  </si>
+  <si>
+    <t>0.9321353</t>
+  </si>
+  <si>
+    <t>0.98051274</t>
+  </si>
+  <si>
+    <t>0.99174285</t>
+  </si>
+  <si>
+    <t>0.9837013</t>
+  </si>
+  <si>
+    <t>0.9491586</t>
+  </si>
+  <si>
+    <t>0.90162235</t>
+  </si>
+  <si>
+    <t>0.80737907</t>
+  </si>
+  <si>
+    <t>0.7173512</t>
+  </si>
+  <si>
+    <t>0.6151961</t>
+  </si>
+  <si>
+    <t>0.44188514</t>
+  </si>
+  <si>
+    <t>0.34071133</t>
+  </si>
+  <si>
+    <t>0.25057378</t>
+  </si>
+  <si>
+    <t>0.19783457</t>
+  </si>
+  <si>
+    <t>0.16634719</t>
+  </si>
+  <si>
+    <t>0.13030091</t>
+  </si>
+  <si>
+    <t>0.10086449</t>
   </si>
 </sst>
 </file>
@@ -526,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04BF92F-29B1-4EF0-A906-3618A0FA08A5}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B23"/>
+      <selection activeCell="B3" sqref="B3:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -558,7 +582,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -566,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -574,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -582,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -590,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -598,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -606,7 +630,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -614,7 +638,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -622,103 +646,127 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12">
-        <v>70</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>